<commit_message>
Update IG-workflows action to use main branch ed2d58a408dc2bda4893b5e293d4ef2ac6de801d
</commit_message>
<xml_diff>
--- a/nriss-patch-1/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/nriss-patch-1/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.1.0</t>
+    <t>2.2.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-19T08:22:07+00:00</t>
+    <t>2025-12-19T09:47:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>